<commit_message>
Update TB for barrelshifter and control
</commit_message>
<xml_diff>
--- a/Control Flow/Proj1_control_signals.xlsx
+++ b/Control Flow/Proj1_control_signals.xlsx
@@ -49,7 +49,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">s_DMemWr </t>
     </r>
@@ -60,7 +59,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[MemWrite from text]</t>
     </r>
@@ -72,7 +70,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">s_RegWr </t>
     </r>
@@ -83,7 +80,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[RegWrite from text]</t>
     </r>
@@ -110,7 +106,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1 </t>
     </r>
@@ -121,7 +116,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[use the appropriately extended immediate as source B]</t>
     </r>
@@ -133,7 +127,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0010 </t>
     </r>
@@ -144,7 +137,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[the alu will perform an add of A and B]</t>
     </r>
@@ -156,7 +148,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0 </t>
     </r>
@@ -167,7 +158,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[addi does NOT read from memory]</t>
     </r>
@@ -179,7 +169,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0 </t>
     </r>
@@ -190,7 +179,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[addi does NOT write to memory]</t>
     </r>
@@ -202,7 +190,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1 </t>
     </r>
@@ -213,7 +200,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[addi writes back to a register]</t>
     </r>
@@ -225,7 +211,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0 </t>
     </r>
@@ -236,7 +221,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[addi uses rt as destination register rather than rd]</t>
     </r>
@@ -402,13 +386,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -424,6 +407,70 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i val="true"/>
@@ -431,24 +478,59 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -456,8 +538,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,6 +578,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -503,19 +648,95 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -526,29 +747,25 @@
   </sheetPr>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:I"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="50.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="46.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="2.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="10.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -573,7 +790,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -599,7 +816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1139,11 +1356,14 @@
       <c r="G28" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H28" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="I28" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>